<commit_message>
Experience with data-driven with Apache POI and jxl
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testdata.xlsx
+++ b/src/test/java/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/IdeaProjects/seleniumnewtours/src/test/java/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD945BE-F585-E24B-8B07-25D30F63D9B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3D1CB5-16B5-0949-AA30-1228A9600843}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15560" xr2:uid="{1F5505D9-47AB-3542-BD97-6D5C7AB7C488}"/>
   </bookViews>
@@ -25,15 +25,216 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
-  <si>
-    <t>mercury</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a8</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>a10</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>b5</t>
+  </si>
+  <si>
+    <t>b6</t>
+  </si>
+  <si>
+    <t>b7</t>
+  </si>
+  <si>
+    <t>b8</t>
+  </si>
+  <si>
+    <t>b9</t>
+  </si>
+  <si>
+    <t>b10</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>c4</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>c6</t>
+  </si>
+  <si>
+    <t>c7</t>
+  </si>
+  <si>
+    <t>c8</t>
+  </si>
+  <si>
+    <t>c9</t>
+  </si>
+  <si>
+    <t>c10</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>e3</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>d4</t>
+  </si>
+  <si>
+    <t>d5</t>
+  </si>
+  <si>
+    <t>d6</t>
+  </si>
+  <si>
+    <t>d7</t>
+  </si>
+  <si>
+    <t>d8</t>
+  </si>
+  <si>
+    <t>d9</t>
+  </si>
+  <si>
+    <t>d10</t>
+  </si>
+  <si>
+    <t>e4</t>
+  </si>
+  <si>
+    <t>e5</t>
+  </si>
+  <si>
+    <t>e6</t>
+  </si>
+  <si>
+    <t>e7</t>
+  </si>
+  <si>
+    <t>e8</t>
+  </si>
+  <si>
+    <t>e9</t>
+  </si>
+  <si>
+    <t>e10</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>f5</t>
+  </si>
+  <si>
+    <t>f6</t>
+  </si>
+  <si>
+    <t>f7</t>
+  </si>
+  <si>
+    <t>f8</t>
+  </si>
+  <si>
+    <t>f9</t>
+  </si>
+  <si>
+    <t>f10</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>g5</t>
+  </si>
+  <si>
+    <t>g6</t>
+  </si>
+  <si>
+    <t>g7</t>
+  </si>
+  <si>
+    <t>g8</t>
+  </si>
+  <si>
+    <t>g9</t>
+  </si>
+  <si>
+    <t>g10</t>
   </si>
 </sst>
 </file>
@@ -385,26 +586,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FC09CE-E2EB-DD46-A56E-D5C7102997E8}">
-  <dimension ref="B1:C2"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data driver with loop
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testdata.xlsx
+++ b/src/test/java/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/IdeaProjects/seleniumnewtours/src/test/java/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BB01F0-71F4-D144-84F3-B5B1A0D05565}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9145826C-27FF-924B-BCCA-B491A1F8B7ED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15560" xr2:uid="{1F5505D9-47AB-3542-BD97-6D5C7AB7C488}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
   <si>
     <t>userName</t>
   </si>
@@ -593,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FC09CE-E2EB-DD46-A56E-D5C7102997E8}">
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,6 +839,238 @@
         <v>54</v>
       </c>
     </row>
+    <row r="3" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Initial parameterization and loop completed.
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testdata.xlsx
+++ b/src/test/java/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/IdeaProjects/seleniumnewtours/src/test/java/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9145826C-27FF-924B-BCCA-B491A1F8B7ED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7A44F3-A5F0-AC48-AE7A-5EFEF4962278}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15560" xr2:uid="{1F5505D9-47AB-3542-BD97-6D5C7AB7C488}"/>
   </bookViews>
@@ -596,7 +596,7 @@
   <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Loop working with 3 different data sets
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testdata.xlsx
+++ b/src/test/java/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/IdeaProjects/seleniumnewtours/src/test/java/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7A44F3-A5F0-AC48-AE7A-5EFEF4962278}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4E86C3-351B-7042-A605-BF857A0A5EDE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15560" xr2:uid="{1F5505D9-47AB-3542-BD97-6D5C7AB7C488}"/>
+    <workbookView xWindow="7200" yWindow="3560" windowWidth="21600" windowHeight="12480" xr2:uid="{1F5505D9-47AB-3542-BD97-6D5C7AB7C488}"/>
   </bookViews>
   <sheets>
     <sheet name="newTours" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
   <si>
     <t>userName</t>
   </si>
@@ -108,21 +108,9 @@
     <t>creditCard</t>
   </si>
   <si>
-    <t>Firstname1</t>
-  </si>
-  <si>
-    <t>Lastname1</t>
-  </si>
-  <si>
     <t>Hindu</t>
   </si>
   <si>
-    <t>Firstname2</t>
-  </si>
-  <si>
-    <t>Lastname2</t>
-  </si>
-  <si>
     <t>Low Calorie</t>
   </si>
   <si>
@@ -165,9 +153,6 @@
     <t>billAddress2</t>
   </si>
   <si>
-    <t>Billing Address Complement</t>
-  </si>
-  <si>
     <t>billCity</t>
   </si>
   <si>
@@ -241,6 +226,177 @@
   </si>
   <si>
     <t>2010</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>UNITED STATES</t>
+  </si>
+  <si>
+    <t>Coach</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Acapulco</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Blue Skies Airlines</t>
+  </si>
+  <si>
+    <t>Pangea Airlines</t>
+  </si>
+  <si>
+    <t>Firstname11</t>
+  </si>
+  <si>
+    <t>Lastname11</t>
+  </si>
+  <si>
+    <t>Firstname21</t>
+  </si>
+  <si>
+    <t>Lastname21</t>
+  </si>
+  <si>
+    <t>Firstname12</t>
+  </si>
+  <si>
+    <t>Lastname12</t>
+  </si>
+  <si>
+    <t>Firstname22</t>
+  </si>
+  <si>
+    <t>Lastname22</t>
+  </si>
+  <si>
+    <t>Firstname13</t>
+  </si>
+  <si>
+    <t>Lastname13</t>
+  </si>
+  <si>
+    <t>Firstname23</t>
+  </si>
+  <si>
+    <t>Lastname23</t>
+  </si>
+  <si>
+    <t>Bland</t>
+  </si>
+  <si>
+    <t>Diabetic</t>
+  </si>
+  <si>
+    <t>Kosher</t>
+  </si>
+  <si>
+    <t>Low Sodium</t>
+  </si>
+  <si>
+    <t>Carte Blanche</t>
+  </si>
+  <si>
+    <t>American Express</t>
+  </si>
+  <si>
+    <t>9238483848</t>
+  </si>
+  <si>
+    <t>4373775834</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2, Billing Address</t>
+  </si>
+  <si>
+    <t>3, Billing Address</t>
+  </si>
+  <si>
+    <t>1, Delivery Address</t>
+  </si>
+  <si>
+    <t>3, Delivery Address</t>
+  </si>
+  <si>
+    <t>Billing Address Complement 1</t>
+  </si>
+  <si>
+    <t>Billing Address Complement 2</t>
+  </si>
+  <si>
+    <t>Billing Address Complement 3</t>
+  </si>
+  <si>
+    <t>1, Delivery Address Complement</t>
+  </si>
+  <si>
+    <t>3, Delivery Address Complement</t>
+  </si>
+  <si>
+    <t>43422</t>
+  </si>
+  <si>
+    <t>34142</t>
+  </si>
+  <si>
+    <t>36563</t>
+  </si>
+  <si>
+    <t>65878</t>
+  </si>
+  <si>
+    <t>BRAZIL</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Gardner</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -596,7 +752,7 @@
   <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,6 +761,7 @@
     <col min="21" max="21" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
@@ -669,58 +826,58 @@
         <v>26</v>
       </c>
       <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" t="s">
         <v>34</v>
       </c>
-      <c r="V1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>45</v>
-      </c>
       <c r="AC1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="AD1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="AE1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AF1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="AG1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>59</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -731,112 +888,112 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="T2" s="1" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="Y2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="AB2" s="1" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="AG2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AL2" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -847,112 +1004,112 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="U3" s="1" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="V3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL3" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -963,112 +1120,112 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="W4" s="1" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="AG4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AH4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AJ4" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>